<commit_message>
add pdfs of tables
</commit_message>
<xml_diff>
--- a/Estimation_Records/1MB regular/1MB regular.xlsx
+++ b/Estimation_Records/1MB regular/1MB regular.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Technion\CommunicationProject\LCCN_Delay_Bit_RTT_Estimator\Estimation_Records\1MB regular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Technion\semester8\delayBit\LCCN_Delay_Bit_RTT_Estimator\Estimation_Records\1MB regular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F3D8B6-5BCD-4791-97C5-03B9C53830CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF17A93-B53C-44F7-A91F-D2FEDC5D2EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FEAB5AA3-3F3A-45DA-9C63-0F6A688FC56D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
   <si>
     <t>Spin bit measurements:</t>
   </si>
@@ -58,12 +61,15 @@
   <si>
     <t>time since initial</t>
   </si>
+  <si>
+    <t xml:space="preserve">Control </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +80,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,10 +112,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -199,7 +213,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-IL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -961,7 +975,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -999,7 +1013,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="519209311"/>
@@ -1084,7 +1098,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1122,7 +1136,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="519198911"/>
@@ -1164,7 +1178,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-IL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1201,7 +1215,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="LID4096"/>
+      <a:endParaRPr lang="en-IL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1296,7 +1310,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-IL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2016,7 +2030,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2054,7 +2068,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="674367695"/>
@@ -2133,7 +2147,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2171,7 +2185,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="674363951"/>
@@ -2219,7 +2233,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="LID4096"/>
+      <a:endParaRPr lang="en-IL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3346,16 +3360,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>77544</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:rowOff>10980</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:rowOff>53787</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3382,16 +3396,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>777240</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>140746</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>71941</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>107</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>107576</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3716,26 +3730,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2173566-75B2-43F4-8EDF-E56C8BE8C964}">
-  <dimension ref="A3:M127"/>
+  <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="2.77734375" customWidth="1"/>
     <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" customWidth="1"/>
     <col min="9" max="9" width="19.109375" customWidth="1"/>
     <col min="10" max="10" width="17.21875" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
     <col min="13" max="13" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
@@ -3746,6 +3766,9 @@
       <c r="D3">
         <v>50.307487000000002</v>
       </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -3836,7 +3859,7 @@
         <v>51.028219</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G9:G56" si="1">F10-$D$3</f>
+        <f t="shared" ref="G10:G56" si="1">F10-$D$3</f>
         <v>0.72073199999999815</v>
       </c>
       <c r="H10">
@@ -4809,6 +4832,9 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="F74" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add q bit records
</commit_message>
<xml_diff>
--- a/Estimation_Records/1MB regular/1MB regular.xlsx
+++ b/Estimation_Records/1MB regular/1MB regular.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Technion\CommunicationProject\LCCN_Delay_Bit_RTT_Estimator\Estimation_Records\1MB regular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Technion\semester8\delayBit\LCCN_Delay_Bit_RTT_Estimator\Estimation_Records\1MB regular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F3D8B6-5BCD-4791-97C5-03B9C53830CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF17A93-B53C-44F7-A91F-D2FEDC5D2EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FEAB5AA3-3F3A-45DA-9C63-0F6A688FC56D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
   <si>
     <t>Spin bit measurements:</t>
   </si>
@@ -58,12 +61,15 @@
   <si>
     <t>time since initial</t>
   </si>
+  <si>
+    <t xml:space="preserve">Control </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +80,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,10 +112,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -199,7 +213,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-IL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -961,7 +975,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -999,7 +1013,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="519209311"/>
@@ -1084,7 +1098,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1122,7 +1136,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="519198911"/>
@@ -1164,7 +1178,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-IL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1201,7 +1215,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="LID4096"/>
+      <a:endParaRPr lang="en-IL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1296,7 +1310,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-IL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2016,7 +2030,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2054,7 +2068,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="674367695"/>
@@ -2133,7 +2147,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2171,7 +2185,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="674363951"/>
@@ -2219,7 +2233,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="LID4096"/>
+      <a:endParaRPr lang="en-IL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3346,16 +3360,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>77544</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:rowOff>10980</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:rowOff>53787</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3382,16 +3396,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>777240</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>140746</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>71941</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>107</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>107576</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3716,26 +3730,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2173566-75B2-43F4-8EDF-E56C8BE8C964}">
-  <dimension ref="A3:M127"/>
+  <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="2.77734375" customWidth="1"/>
     <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" customWidth="1"/>
     <col min="9" max="9" width="19.109375" customWidth="1"/>
     <col min="10" max="10" width="17.21875" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
     <col min="13" max="13" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
@@ -3746,6 +3766,9 @@
       <c r="D3">
         <v>50.307487000000002</v>
       </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -3836,7 +3859,7 @@
         <v>51.028219</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G9:G56" si="1">F10-$D$3</f>
+        <f t="shared" ref="G10:G56" si="1">F10-$D$3</f>
         <v>0.72073199999999815</v>
       </c>
       <c r="H10">
@@ -4809,6 +4832,9 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="F74" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>